<commit_message>
GUI now displays Red Line schedule generated from Excel file
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/schedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/schedule.xlsx
@@ -5,22 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\GitHub\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
-    <sheet name="Train" sheetId="7" r:id="rId2"/>
+    <sheet name="Red" sheetId="7" r:id="rId2"/>
+    <sheet name="Green" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
   <si>
     <t>Monday</t>
   </si>
@@ -76,40 +78,67 @@
     <t>Train ID</t>
   </si>
   <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>Track Section</t>
-  </si>
-  <si>
-    <t>Block</t>
-  </si>
-  <si>
-    <t>Next Station</t>
-  </si>
-  <si>
-    <t>Time of Arrival</t>
-  </si>
-  <si>
-    <t>Authority</t>
-  </si>
-  <si>
-    <t>Current Speed</t>
-  </si>
-  <si>
-    <t>Suggested</t>
-  </si>
-  <si>
-    <t>Passengers</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
     <t xml:space="preserve">OFF </t>
+  </si>
+  <si>
+    <t>SHADYSIDE</t>
+  </si>
+  <si>
+    <t>HERRON</t>
+  </si>
+  <si>
+    <t>SWISSVILLE</t>
+  </si>
+  <si>
+    <t>STEEL PLAZA</t>
+  </si>
+  <si>
+    <t>PENN STATION</t>
+  </si>
+  <si>
+    <t>FIRST AVE</t>
+  </si>
+  <si>
+    <t>ST SQUARE</t>
+  </si>
+  <si>
+    <t>STH HILLS</t>
+  </si>
+  <si>
+    <t>DRIVER</t>
+  </si>
+  <si>
+    <t>Employee A</t>
+  </si>
+  <si>
+    <t>Employee B</t>
+  </si>
+  <si>
+    <t>Employee C</t>
+  </si>
+  <si>
+    <t>Employee D</t>
+  </si>
+  <si>
+    <t>Employee E</t>
+  </si>
+  <si>
+    <t>DEPARTURE</t>
+  </si>
+  <si>
+    <t>06.00.00</t>
+  </si>
+  <si>
+    <t>06.15.00</t>
+  </si>
+  <si>
+    <t>06.30.00</t>
+  </si>
+  <si>
+    <t>06.45.00</t>
+  </si>
+  <si>
+    <t>07.00.00</t>
   </si>
 </sst>
 </file>
@@ -159,11 +188,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -700,7 +731,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -720,16 +751,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
@@ -738,84 +769,384 @@
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>104</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>105</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.25486111111111109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.26041666666666669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.26527777777777778</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <f>C2+TIME(0,3.7,0)</f>
+        <v>0.25208333333333333</v>
+      </c>
+      <c r="E7" s="2">
+        <f>D7+TIME(0,2.3,0)</f>
+        <v>0.25347222222222221</v>
+      </c>
+      <c r="F7" s="2">
+        <f>E7+TIME(0,1.5,0)</f>
+        <v>0.25416666666666665</v>
+      </c>
+      <c r="G7" s="2">
+        <f>F7+TIME(0,1.8,0)</f>
+        <v>0.25486111111111109</v>
+      </c>
+      <c r="H7" s="2">
+        <f>G7+TIME(0,2.1,0)</f>
+        <v>0.25624999999999998</v>
+      </c>
+      <c r="I7" s="2">
+        <f>H7+TIME(0,2.1,0)</f>
+        <v>0.25763888888888886</v>
+      </c>
+      <c r="J7" s="2">
+        <f>I7+TIME(0,1.7,0)</f>
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="K7" s="2">
+        <f>J7+TIME(0,2.3,0)</f>
+        <v>0.25972222222222219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f>C3+TIME(0,3.7,0)</f>
+        <v>0.25694444444444442</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" ref="E8:E11" si="0">D8+TIME(0,2.3,0)</f>
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" ref="F8:F11" si="1">E8+TIME(0,1.5,0)</f>
+        <v>0.25902777777777775</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8:G11" si="2">F8+TIME(0,1.8,0)</f>
+        <v>0.25972222222222219</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8:I11" si="3">G8+TIME(0,2.1,0)</f>
+        <v>0.26111111111111107</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26249999999999996</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" ref="J8:J11" si="4">I8+TIME(0,1.7,0)</f>
+        <v>0.2631944444444444</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" ref="K8:K11" si="5">J8+TIME(0,2.3,0)</f>
+        <v>0.26458333333333328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <f>C4+TIME(0,3.7,0)</f>
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2638888888888889</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.26458333333333334</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.26527777777777778</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.26805555555555555</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.26874999999999999</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="5"/>
+        <v>0.27013888888888887</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f>C5+TIME(0,3.7,0)</f>
+        <v>0.2673611111111111</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.26874999999999999</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.26944444444444443</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.27013888888888887</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27152777777777776</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.27361111111111108</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="5"/>
+        <v>0.27499999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f>C6+TIME(0,3.7,0)</f>
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.27430555555555552</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.27569444444444441</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27708333333333329</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.27847222222222218</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="4"/>
+        <v>0.27916666666666662</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="5"/>
+        <v>0.2805555555555555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Functionality for uploading schedules and updating train dropdown box added
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/schedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/schedule.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
     <sheet name="Red" sheetId="7" r:id="rId2"/>
     <sheet name="Green" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
   <si>
     <t>Monday</t>
   </si>
@@ -139,12 +139,15 @@
   </si>
   <si>
     <t>07.00.00</t>
+  </si>
+  <si>
+    <t>OFF2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,13 +191,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,23 +292,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -340,23 +327,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -535,9 +505,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +562,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -753,9 +723,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +781,7 @@
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made employee naming convention uniform across all schedules
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/schedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
   <si>
     <t>Monday</t>
   </si>
@@ -48,27 +48,9 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>Employee 1</t>
-  </si>
-  <si>
     <t>OFF</t>
   </si>
   <si>
-    <t>Employee 2</t>
-  </si>
-  <si>
-    <t>Employee 3</t>
-  </si>
-  <si>
-    <t>Employee 4</t>
-  </si>
-  <si>
-    <t>Employee 5</t>
-  </si>
-  <si>
-    <t>Employee 6</t>
-  </si>
-  <si>
     <t>6am - 2:30pm</t>
   </si>
   <si>
@@ -142,6 +124,12 @@
   </si>
   <si>
     <t>OFF2</t>
+  </si>
+  <si>
+    <t>Employee F</t>
+  </si>
+  <si>
+    <t>Employee G</t>
   </si>
 </sst>
 </file>
@@ -507,31 +495,31 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -557,160 +545,160 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -728,108 +716,108 @@
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>104</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C7" s="3"/>
     </row>
   </sheetData>
@@ -846,110 +834,110 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2">
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2">
         <v>0.25486111111111109</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2">
         <v>0.26041666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2">
         <v>0.26527777777777778</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>0.27083333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D7" s="2">
         <f>C2+TIME(0,3.7,0)</f>
         <v>0.25208333333333333</v>
@@ -983,7 +971,7 @@
         <v>0.25972222222222219</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D8" s="2">
         <f>C3+TIME(0,3.7,0)</f>
         <v>0.25694444444444442</v>
@@ -1017,7 +1005,7 @@
         <v>0.26458333333333328</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D9" s="2">
         <f>C4+TIME(0,3.7,0)</f>
         <v>0.26250000000000001</v>
@@ -1051,7 +1039,7 @@
         <v>0.27013888888888887</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D10" s="2">
         <f>C5+TIME(0,3.7,0)</f>
         <v>0.2673611111111111</v>
@@ -1085,7 +1073,7 @@
         <v>0.27499999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D11" s="2">
         <f>C6+TIME(0,3.7,0)</f>
         <v>0.27291666666666664</v>

</xml_diff>

<commit_message>
Schedule fixed (for real)
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/schedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/schedule.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\GitHub\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
     <sheet name="Red" sheetId="7" r:id="rId2"/>
     <sheet name="Green" sheetId="8" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
@@ -108,12 +108,6 @@
     <t>DEPARTURE</t>
   </si>
   <si>
-    <t>06.00.00</t>
-  </si>
-  <si>
-    <t>06.15.00</t>
-  </si>
-  <si>
     <t>Employee 1</t>
   </si>
   <si>
@@ -132,22 +126,28 @@
     <t>Employee 6</t>
   </si>
   <si>
-    <t>14.00.00</t>
-  </si>
-  <si>
-    <t>14.15.00</t>
-  </si>
-  <si>
-    <t>14.30.00</t>
-  </si>
-  <si>
     <t>06.30.00</t>
+  </si>
+  <si>
+    <t>06.10.00</t>
+  </si>
+  <si>
+    <t>06.01.00</t>
+  </si>
+  <si>
+    <t>06.20.00</t>
+  </si>
+  <si>
+    <t>06.40.00</t>
+  </si>
+  <si>
+    <t>06.50.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,23 +291,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -343,23 +326,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -543,28 +509,28 @@
       <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -590,9 +556,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -616,9 +582,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -642,9 +608,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -668,9 +634,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -694,9 +660,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -720,9 +686,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -758,21 +724,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -807,70 +773,70 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -887,20 +853,20 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -935,7 +901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
@@ -946,7 +912,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101</v>
       </c>
@@ -957,7 +923,7 @@
         <v>0.25486111111111109</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102</v>
       </c>
@@ -968,7 +934,7 @@
         <v>0.26041666666666669</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103</v>
       </c>
@@ -979,7 +945,7 @@
         <v>0.26527777777777778</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>104</v>
       </c>
@@ -990,7 +956,7 @@
         <v>0.27083333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D7" s="2">
         <f>C2+TIME(0,3.7,0)</f>
         <v>0.25208333333333333</v>
@@ -1024,7 +990,7 @@
         <v>0.25972222222222219</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D8" s="2">
         <f>C3+TIME(0,3.7,0)</f>
         <v>0.25694444444444442</v>
@@ -1058,7 +1024,7 @@
         <v>0.26458333333333328</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D9" s="2">
         <f>C4+TIME(0,3.7,0)</f>
         <v>0.26250000000000001</v>
@@ -1092,7 +1058,7 @@
         <v>0.27013888888888887</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D10" s="2">
         <f>C5+TIME(0,3.7,0)</f>
         <v>0.2673611111111111</v>
@@ -1126,7 +1092,7 @@
         <v>0.27499999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D11" s="2">
         <f>C6+TIME(0,3.7,0)</f>
         <v>0.27291666666666664</v>

</xml_diff>

<commit_message>
Scheduling works better now
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/schedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
   <si>
     <t>Monday</t>
   </si>
@@ -90,21 +90,6 @@
     <t>DRIVER</t>
   </si>
   <si>
-    <t>Employee A</t>
-  </si>
-  <si>
-    <t>Employee B</t>
-  </si>
-  <si>
-    <t>Employee C</t>
-  </si>
-  <si>
-    <t>Employee D</t>
-  </si>
-  <si>
-    <t>Employee E</t>
-  </si>
-  <si>
     <t>DEPARTURE</t>
   </si>
   <si>
@@ -142,6 +127,57 @@
   </si>
   <si>
     <t>06.50.00</t>
+  </si>
+  <si>
+    <t>Employee 7</t>
+  </si>
+  <si>
+    <t>Employee 8</t>
+  </si>
+  <si>
+    <t>Employee 9</t>
+  </si>
+  <si>
+    <t>Employee 10</t>
+  </si>
+  <si>
+    <t>PIONEER</t>
+  </si>
+  <si>
+    <t>EDGEBROOK</t>
+  </si>
+  <si>
+    <t>PITT</t>
+  </si>
+  <si>
+    <t>WHITED</t>
+  </si>
+  <si>
+    <t>SOUTH BANK</t>
+  </si>
+  <si>
+    <t>CENTRAL</t>
+  </si>
+  <si>
+    <t>INGLEWOOD</t>
+  </si>
+  <si>
+    <t>OVERBROOK</t>
+  </si>
+  <si>
+    <t>GLENBURY</t>
+  </si>
+  <si>
+    <t>DORMONT</t>
+  </si>
+  <si>
+    <t>MT LEBANON</t>
+  </si>
+  <si>
+    <t>POPLAR</t>
+  </si>
+  <si>
+    <t>CASTLE SHANON</t>
   </si>
 </sst>
 </file>
@@ -558,7 +594,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -584,7 +620,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -610,7 +646,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -636,7 +672,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -662,7 +698,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -688,7 +724,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -722,9 +758,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,7 +782,7 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -778,10 +814,10 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -789,10 +825,10 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -800,10 +836,10 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -811,10 +847,10 @@
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -822,10 +858,10 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -833,10 +869,10 @@
         <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -847,14 +883,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" customWidth="1"/>
@@ -866,7 +903,7 @@
     <col min="11" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -874,257 +911,167 @@
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.25486111111111109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.26041666666666669</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.26527777777777778</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.27083333333333331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D7" s="2">
-        <f>C2+TIME(0,3.7,0)</f>
-        <v>0.25208333333333333</v>
-      </c>
-      <c r="E7" s="2">
-        <f>D7+TIME(0,2.3,0)</f>
-        <v>0.25347222222222221</v>
-      </c>
-      <c r="F7" s="2">
-        <f>E7+TIME(0,1.5,0)</f>
-        <v>0.25416666666666665</v>
-      </c>
-      <c r="G7" s="2">
-        <f>F7+TIME(0,1.8,0)</f>
-        <v>0.25486111111111109</v>
-      </c>
-      <c r="H7" s="2">
-        <f>G7+TIME(0,2.1,0)</f>
-        <v>0.25624999999999998</v>
-      </c>
-      <c r="I7" s="2">
-        <f>H7+TIME(0,2.1,0)</f>
-        <v>0.25763888888888886</v>
-      </c>
-      <c r="J7" s="2">
-        <f>I7+TIME(0,1.7,0)</f>
-        <v>0.2583333333333333</v>
-      </c>
-      <c r="K7" s="2">
-        <f>J7+TIME(0,2.3,0)</f>
-        <v>0.25972222222222219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D8" s="2">
-        <f>C3+TIME(0,3.7,0)</f>
-        <v>0.25694444444444442</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" ref="E8:E11" si="0">D8+TIME(0,2.3,0)</f>
-        <v>0.2583333333333333</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" ref="F8:F11" si="1">E8+TIME(0,1.5,0)</f>
-        <v>0.25902777777777775</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" ref="G8:G11" si="2">F8+TIME(0,1.8,0)</f>
-        <v>0.25972222222222219</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" ref="H8:I11" si="3">G8+TIME(0,2.1,0)</f>
-        <v>0.26111111111111107</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="3"/>
-        <v>0.26249999999999996</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" ref="J8:J11" si="4">I8+TIME(0,1.7,0)</f>
-        <v>0.2631944444444444</v>
-      </c>
-      <c r="K8" s="2">
-        <f t="shared" ref="K8:K11" si="5">J8+TIME(0,2.3,0)</f>
-        <v>0.26458333333333328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D9" s="2">
-        <f>C4+TIME(0,3.7,0)</f>
-        <v>0.26250000000000001</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.2638888888888889</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="1"/>
-        <v>0.26458333333333334</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="2"/>
-        <v>0.26527777777777778</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" si="3"/>
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="3"/>
-        <v>0.26805555555555555</v>
-      </c>
-      <c r="J9" s="2">
-        <f t="shared" si="4"/>
-        <v>0.26874999999999999</v>
-      </c>
-      <c r="K9" s="2">
-        <f t="shared" si="5"/>
-        <v>0.27013888888888887</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D10" s="2">
-        <f>C5+TIME(0,3.7,0)</f>
-        <v>0.2673611111111111</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.26874999999999999</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="1"/>
-        <v>0.26944444444444443</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="2"/>
-        <v>0.27013888888888887</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" si="3"/>
-        <v>0.27152777777777776</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="3"/>
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="J10" s="2">
-        <f t="shared" si="4"/>
-        <v>0.27361111111111108</v>
-      </c>
-      <c r="K10" s="2">
-        <f t="shared" si="5"/>
-        <v>0.27499999999999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D11" s="2">
-        <f>C6+TIME(0,3.7,0)</f>
-        <v>0.27291666666666664</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.27430555555555552</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.27499999999999997</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="2"/>
-        <v>0.27569444444444441</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="3"/>
-        <v>0.27708333333333329</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="3"/>
-        <v>0.27847222222222218</v>
-      </c>
-      <c r="J11" s="2">
-        <f t="shared" si="4"/>
-        <v>0.27916666666666662</v>
-      </c>
-      <c r="K11" s="2">
-        <f t="shared" si="5"/>
-        <v>0.2805555555555555</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added getter methods for Inglewood inbound and Central inbound times
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/schedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/schedule.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Documents\GitHub\ECE1186\TrainSystem\src\com\rogueone\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9036"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9030" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
@@ -78,36 +78,12 @@
     <t>Employee 6</t>
   </si>
   <si>
-    <t>06.30.00</t>
-  </si>
-  <si>
     <t>06.10.00</t>
   </si>
   <si>
-    <t>06.01.00</t>
-  </si>
-  <si>
-    <t>06.20.00</t>
-  </si>
-  <si>
     <t>06.40.00</t>
   </si>
   <si>
-    <t>06.50.00</t>
-  </si>
-  <si>
-    <t>Employee 7</t>
-  </si>
-  <si>
-    <t>Employee 8</t>
-  </si>
-  <si>
-    <t>Employee 9</t>
-  </si>
-  <si>
-    <t>Employee 10</t>
-  </si>
-  <si>
     <t>PIONEER</t>
   </si>
   <si>
@@ -220,12 +196,24 @@
   </si>
   <si>
     <t>3:20pm</t>
+  </si>
+  <si>
+    <t>06.25.00</t>
+  </si>
+  <si>
+    <t>06.55.00</t>
+  </si>
+  <si>
+    <t>07.10.00</t>
+  </si>
+  <si>
+    <t>07.25.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,6 +357,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -404,6 +409,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -582,149 +604,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -739,21 +761,21 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C7"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -788,70 +810,70 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>104</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -864,25 +886,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -893,116 +915,125 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>107</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>108</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>109</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>110</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1012,7 +1043,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -1022,7 +1053,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1032,7 +1063,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1042,7 +1073,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>

</xml_diff>